<commit_message>
Add employee page in progress
</commit_message>
<xml_diff>
--- a/OrangeHRM_Project/src/test/resources/TestData/Locator_Data.xlsx
+++ b/OrangeHRM_Project/src/test/resources/TestData/Locator_Data.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AutomationTesting\OrangeHRM_Project\src\test\resources\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AutomationTesting\OrangeHRM_Project\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="LoginPage" sheetId="1" r:id="rId1"/>
@@ -253,7 +253,13 @@
     <t>select_photo</t>
   </si>
   <si>
-    <t>//input[@type='file'][@class='oxd-file-input']</t>
+    <t>input[type='file']</t>
+  </si>
+  <si>
+    <t>//input[@type='file']</t>
+  </si>
+  <si>
+    <t>oxd-file-input</t>
   </si>
   <si>
     <t>addEmp_heading</t>
@@ -633,8 +639,8 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -794,8 +800,8 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -999,8 +1005,14 @@
       <c r="A10" s="2" t="s">
         <v>76</v>
       </c>
+      <c r="D10" s="3" t="s">
+        <v>77</v>
+      </c>
       <c r="E10" s="3" t="s">
-        <v>77</v>
+        <v>78</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>79</v>
       </c>
       <c r="G10" s="2" t="s">
         <v>14</v>
@@ -1008,19 +1020,19 @@
     </row>
     <row r="11" ht="28.8">
       <c r="A11" s="2" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>

</xml_diff>